<commit_message>
MT-v2.6: Next: manage banner, facebook, g+
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -19,33 +19,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Hoa</t>
-  </si>
-  <si>
-    <t>Nguyen</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+  <si>
+    <t>product_id</t>
+  </si>
+  <si>
+    <t>category_id</t>
+  </si>
+  <si>
+    <t>tax_id</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>specifications</t>
+  </si>
+  <si>
+    <t>is_discount</t>
+  </si>
+  <si>
+    <t>is_highlight</t>
+  </si>
+  <si>
+    <t>Máy chấm công mới</t>
+  </si>
+  <si>
+    <t>Máy chấm công mới A</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -69,8 +102,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,48 +385,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
       <c r="C2">
-        <v>123</v>
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>200000</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
         <v>4</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
       <c r="C3">
-        <v>234</v>
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>400000</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>